<commit_message>
apply create char arrange json file
</commit_message>
<xml_diff>
--- a/BlueServer/json/SimTable.xlsx
+++ b/BlueServer/json/SimTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\GO_WORK\bin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Blue\BlueServer\trunk\BlueServerLinux\BlueServer\json\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
   <si>
     <t>TableName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -272,15 +272,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>CreateWarrior</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateArcher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VCType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>VC2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CreateWarrior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateArcher</t>
+    <t>Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1179,34 +1187,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -1214,10 +1223,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>56</v>
       </c>
@@ -1225,28 +1237,37 @@
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="2">
+        <v>61</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="4">
+        <v>62</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="4">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
apply levelup, tier up add vs filter
</commit_message>
<xml_diff>
--- a/BlueServer/json/SimTable.xlsx
+++ b/BlueServer/json/SimTable.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24090" windowHeight="10785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24090" windowHeight="10785" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Char" sheetId="1" r:id="rId1"/>
     <sheet name="Product" sheetId="11" r:id="rId2"/>
-    <sheet name="warriorStat" sheetId="2" r:id="rId3"/>
+    <sheet name="WarriorStat" sheetId="2" r:id="rId3"/>
     <sheet name="ArcherStat" sheetId="3" r:id="rId4"/>
     <sheet name="CharTier" sheetId="4" r:id="rId5"/>
     <sheet name="DungeonTier" sheetId="10" r:id="rId6"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="68">
   <si>
     <t>TableName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -65,18 +65,6 @@
     <t>Archer</t>
   </si>
   <si>
-    <t>MonsterA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MonsterB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MonsterC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Level</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -272,14 +260,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CreateWarrior</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CreateArcher</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VCType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -289,6 +269,34 @@
   </si>
   <si>
     <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProductCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CreateChar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CharNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UInt32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MobC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MobB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MobA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -764,7 +772,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -791,24 +799,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -838,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -849,7 +857,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -860,7 +868,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -877,8 +885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -894,7 +902,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -904,48 +912,48 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -953,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -976,7 +984,7 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -999,7 +1007,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -1022,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4">
         <v>4</v>
@@ -1045,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -1068,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="4">
         <v>6</v>
@@ -1091,7 +1099,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2">
         <v>7</v>
@@ -1114,7 +1122,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4">
         <v>8</v>
@@ -1137,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2">
         <v>9</v>
@@ -1160,7 +1168,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4">
         <v>10</v>
@@ -1187,87 +1195,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" customWidth="1"/>
+    <col min="3" max="4" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="2">
+        <v>62</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" s="4">
         <v>1000</v>
       </c>
     </row>
@@ -1282,7 +1302,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1297,7 +1317,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1307,36 +1327,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1705,7 +1725,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1715,36 +1735,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2117,7 +2137,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2127,48 +2147,48 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2176,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2191,10 +2211,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -2206,10 +2226,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2221,16 +2241,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="6"/>
@@ -2240,16 +2260,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
@@ -2259,16 +2279,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="6"/>
@@ -2278,22 +2298,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="G14" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2301,22 +2321,22 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2324,22 +2344,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +2392,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -2382,48 +2402,48 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -2431,10 +2451,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -2446,10 +2466,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -2461,10 +2481,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2476,16 +2496,16 @@
         <v>4</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="6"/>
@@ -2495,16 +2515,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
@@ -2514,16 +2534,16 @@
         <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F13" s="4"/>
       <c r="G13" s="6"/>
@@ -2533,22 +2553,22 @@
         <v>7</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2556,22 +2576,22 @@
         <v>8</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2579,22 +2599,22 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2623,7 +2643,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2633,36 +2653,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -2991,7 +3011,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3001,36 +3021,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3359,7 +3379,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3369,36 +3389,36 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>